<commit_message>
Gathered some more data
</commit_message>
<xml_diff>
--- a/project2/Data/weeklyincome_occupation_gender_2018.xlsx
+++ b/project2/Data/weeklyincome_occupation_gender_2018.xlsx
@@ -1808,12 +1808,12 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2097,7 +2097,7 @@
   <dimension ref="A1:G573"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2106,8 +2106,8 @@
     <col min="2" max="7" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -15176,13 +15176,13 @@
       <c r="G572" s="9"/>
     </row>
     <row r="573" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A573" s="11"/>
-      <c r="B573" s="12"/>
-      <c r="C573" s="12"/>
-      <c r="D573" s="12"/>
-      <c r="E573" s="12"/>
-      <c r="F573" s="12"/>
-      <c r="G573" s="12"/>
+      <c r="A573" s="12"/>
+      <c r="B573" s="13"/>
+      <c r="C573" s="13"/>
+      <c r="D573" s="13"/>
+      <c r="E573" s="13"/>
+      <c r="F573" s="13"/>
+      <c r="G573" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>